<commit_message>
Fixed getting Kafka relations and added four projects.
</commit_message>
<xml_diff>
--- a/data/mall-swarm/mall-auth_structure.xlsx
+++ b/data/mall-swarm/mall-auth_structure.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="181">
   <si>
     <t>Class Name</t>
   </si>
@@ -387,85 +387,85 @@
     <t>Field Type</t>
   </si>
   <si>
+    <t>ACCOUNT_EXPIRED</t>
+  </si>
+  <si>
+    <t>CREDENTIALS_EXPIRED</t>
+  </si>
+  <si>
+    <t>USERNAME_PASSWORD_ERROR</t>
+  </si>
+  <si>
+    <t>PERMISSION_DENIED</t>
+  </si>
+  <si>
+    <t>ACCOUNT_DISABLED</t>
+  </si>
+  <si>
+    <t>ACCOUNT_LOCKED</t>
+  </si>
+  <si>
     <t>LOGIN_SUCCESS</t>
   </si>
   <si>
-    <t>PERMISSION_DENIED</t>
-  </si>
-  <si>
-    <t>ACCOUNT_DISABLED</t>
-  </si>
-  <si>
-    <t>USERNAME_PASSWORD_ERROR</t>
-  </si>
-  <si>
-    <t>ACCOUNT_LOCKED</t>
-  </si>
-  <si>
-    <t>CREDENTIALS_EXPIRED</t>
-  </si>
-  <si>
-    <t>ACCOUNT_EXPIRED</t>
-  </si>
-  <si>
     <t>tokenEndpoint</t>
   </si>
   <si>
     <t>org.springframework.security.oauth2.provider.endpoint.TokenEndpoint</t>
   </si>
   <si>
+    <t>passwordEncoder</t>
+  </si>
+  <si>
+    <t>authenticationManager</t>
+  </si>
+  <si>
+    <t>userDetailsService</t>
+  </si>
+  <si>
     <t>jwtTokenEnhancer</t>
   </si>
   <si>
-    <t>authenticationManager</t>
-  </si>
-  <si>
-    <t>passwordEncoder</t>
-  </si>
-  <si>
-    <t>userDetailsService</t>
+    <t>refreshToken</t>
   </si>
   <si>
     <t>tokenHead</t>
   </si>
   <si>
+    <t>expiresIn</t>
+  </si>
+  <si>
     <t>token</t>
   </si>
   <si>
-    <t>refreshToken</t>
-  </si>
-  <si>
-    <t>expiresIn</t>
+    <t>memberService</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>javax.servlet.http.HttpServletRequest</t>
   </si>
   <si>
     <t>adminService</t>
   </si>
   <si>
-    <t>request</t>
-  </si>
-  <si>
-    <t>javax.servlet.http.HttpServletRequest</t>
-  </si>
-  <si>
-    <t>memberService</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>clientId</t>
   </si>
   <si>
     <t>authorities</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>clientId</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>enabled</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
   <si>
     <t>keyPair</t>
@@ -3311,7 +3311,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3440,24 +3440,24 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14">
@@ -3465,7 +3465,7 @@
         <v>50</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>167</v>
@@ -3473,10 +3473,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>167</v>
@@ -3487,7 +3487,7 @@
         <v>56</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>167</v>
@@ -3498,7 +3498,7 @@
         <v>56</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>167</v>
@@ -3509,7 +3509,7 @@
         <v>56</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>167</v>
@@ -3520,7 +3520,7 @@
         <v>56</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>167</v>
@@ -3531,7 +3531,7 @@
         <v>56</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>167</v>
@@ -3542,7 +3542,7 @@
         <v>56</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>167</v>
@@ -3553,7 +3553,7 @@
         <v>56</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>167</v>
@@ -3564,7 +3564,7 @@
         <v>56</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>167</v>
@@ -3575,7 +3575,7 @@
         <v>56</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>167</v>
@@ -3586,10 +3586,10 @@
         <v>56</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26">
@@ -3597,10 +3597,10 @@
         <v>56</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27">
@@ -3608,43 +3608,43 @@
         <v>56</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31">
@@ -3652,7 +3652,7 @@
         <v>65</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>176</v>
@@ -3663,7 +3663,7 @@
         <v>65</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>176</v>
@@ -3674,7 +3674,7 @@
         <v>65</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s" s="0">
         <v>176</v>
@@ -3685,10 +3685,10 @@
         <v>65</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35">
@@ -3696,7 +3696,7 @@
         <v>65</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>167</v>
@@ -3704,24 +3704,24 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>155</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38">
@@ -3729,7 +3729,7 @@
         <v>84</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s" s="0">
         <v>167</v>
@@ -3740,7 +3740,7 @@
         <v>84</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s" s="0">
         <v>167</v>
@@ -3751,7 +3751,7 @@
         <v>84</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s" s="0">
         <v>167</v>
@@ -3762,7 +3762,7 @@
         <v>84</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s" s="0">
         <v>167</v>
@@ -3773,7 +3773,7 @@
         <v>84</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s" s="0">
         <v>167</v>
@@ -3784,7 +3784,7 @@
         <v>84</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C43" t="s" s="0">
         <v>167</v>
@@ -3795,7 +3795,7 @@
         <v>84</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C44" t="s" s="0">
         <v>167</v>
@@ -3806,7 +3806,7 @@
         <v>84</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s" s="0">
         <v>167</v>
@@ -3817,7 +3817,7 @@
         <v>84</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s" s="0">
         <v>167</v>
@@ -3828,7 +3828,7 @@
         <v>84</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s" s="0">
         <v>167</v>
@@ -3839,7 +3839,7 @@
         <v>84</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C48" t="s" s="0">
         <v>167</v>
@@ -3850,7 +3850,7 @@
         <v>84</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s" s="0">
         <v>167</v>
@@ -3861,7 +3861,7 @@
         <v>84</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C50" t="s" s="0">
         <v>167</v>
@@ -3872,7 +3872,7 @@
         <v>84</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s" s="0">
         <v>167</v>
@@ -3883,7 +3883,7 @@
         <v>84</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s" s="0">
         <v>167</v>
@@ -3894,10 +3894,10 @@
         <v>84</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54">
@@ -3905,10 +3905,10 @@
         <v>84</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55">
@@ -3916,10 +3916,10 @@
         <v>84</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56">
@@ -3927,10 +3927,10 @@
         <v>84</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57">
@@ -3938,20 +3938,31 @@
         <v>84</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
         <v>114</v>
       </c>
-      <c r="B58" t="s" s="0">
+      <c r="B59" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="C58" t="s" s="0">
+      <c r="C59" t="s" s="0">
         <v>175</v>
       </c>
     </row>
@@ -4440,7 +4451,7 @@
         <v>93</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11">
@@ -4468,7 +4479,7 @@
         <v>93</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>54</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
@@ -4482,7 +4493,7 @@
         <v>93</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>74</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14">
@@ -4524,7 +4535,7 @@
         <v>93</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
@@ -4538,7 +4549,7 @@
         <v>93</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -4552,7 +4563,7 @@
         <v>93</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -4580,7 +4591,7 @@
         <v>93</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21">
@@ -4602,13 +4613,13 @@
         <v>65</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>93</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
@@ -4622,7 +4633,7 @@
         <v>93</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
@@ -4630,7 +4641,7 @@
         <v>65</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>93</v>
@@ -4650,7 +4661,7 @@
         <v>93</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26">
@@ -4664,7 +4675,7 @@
         <v>93</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>96</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -4678,7 +4689,7 @@
         <v>93</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>13</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28">
@@ -4706,7 +4717,7 @@
         <v>93</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>89</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
@@ -4720,7 +4731,7 @@
         <v>93</v>
       </c>
       <c r="D30" t="s" s="0">
-        <v>13</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31">

</xml_diff>